<commit_message>
Corrected data types, formatted the data placeholder to  number for Unknown value for all fields
</commit_message>
<xml_diff>
--- a/Dimension Tables/Payment Type.xlsx
+++ b/Dimension Tables/Payment Type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\PowerBI Projects\NYC Trips Project\NYC-Trips-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\PowerBI Projects\Trips Project\NYC-Trips-Project\Dimension Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8AAAE4-8B9D-4173-800A-A6B1B19C6D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9850FE-370E-4B2C-9541-4E5B179283EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41180A30-2EF3-43BA-B41A-9DAB92B33034}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Type</t>
   </si>
@@ -135,8 +135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{642832BD-87C9-452D-B4F1-DABEEA777ED6}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{642832BD-87C9-452D-B4F1-DABEEA777ED6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{642832BD-87C9-452D-B4F1-DABEEA777ED6}" name="Table1" displayName="Table1" ref="A1:B8" totalsRowShown="0">
+  <autoFilter ref="A1:B8" xr:uid="{642832BD-87C9-452D-B4F1-DABEEA777ED6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{26E3E9B1-F90C-43DA-BE82-926F1537CED8}" name="Type"/>
     <tableColumn id="2" xr3:uid="{480347A3-3C24-49F6-A23C-022B4404EA5F}" name="Name"/>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B42C8AF-FC9E-4AE2-9EE6-7FDE7845327D}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,6 +531,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>